<commit_message>
Effects wil be displayed
</commit_message>
<xml_diff>
--- a/data/datasets/base/base_ds.xlsx
+++ b/data/datasets/base/base_ds.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\Me\GitHub\KYC\data\datasets\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83194019-20F9-47E3-8420-FB74C22058A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29A2E23-3C70-4275-B77A-7BC2C6CADFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{EFC702AD-A6EF-45FA-930B-3A40216C84F8}"/>
   </bookViews>
@@ -1879,7 +1879,7 @@
   <dimension ref="A1:S70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1888,17 +1888,17 @@
     <col min="3" max="3" width="18.5703125" style="1" customWidth="1"/>
     <col min="4" max="5" width="13.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="1" customWidth="1"/>
-    <col min="7" max="7" width="40" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="38.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="28" style="1" customWidth="1"/>
-    <col min="16" max="18" width="13.140625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="130" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="1" customWidth="1"/>
+    <col min="13" max="15" width="13.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="130" style="1" customWidth="1"/>
+    <col min="17" max="17" width="40" style="1" customWidth="1"/>
+    <col min="18" max="18" width="38.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="28" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -1921,43 +1921,43 @@
         <v>156</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -1980,28 +1980,28 @@
         <v>227</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="H2" s="1">
+        <v>30</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="I2" s="1">
-        <v>30</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -2024,28 +2024,28 @@
         <v>234</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -2064,38 +2064,38 @@
       <c r="E4" s="1">
         <v>120</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>237</v>
       </c>
+      <c r="I4" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="J4" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="K4" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="K4" s="1">
+        <v>80</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="M4" s="1">
-        <v>80</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -2118,31 +2118,31 @@
         <v>242</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="H5" s="1">
+        <v>100</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="I5" s="1">
-        <v>100</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="R5" t="s">
         <v>245</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -2161,35 +2161,35 @@
       <c r="E6" s="1">
         <v>40</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="I6" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="J6" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="K6" t="s">
+      <c r="P6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="R6" t="s">
         <v>248</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="O6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -2208,38 +2208,38 @@
       <c r="E7" s="1">
         <v>100</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="I7" s="1">
+      <c r="H7" s="1">
         <v>50</v>
       </c>
+      <c r="I7" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="J7" s="1" t="s">
-        <v>177</v>
+        <v>9</v>
+      </c>
+      <c r="K7" s="1">
+        <v>40</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M7" s="1">
-        <v>40</v>
+        <v>178</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="O7" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -2258,31 +2258,31 @@
       <c r="E8" s="1">
         <v>70</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="I8" s="1">
+      <c r="H8" s="1">
         <v>20</v>
       </c>
+      <c r="I8" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="J8" s="1" t="s">
-        <v>189</v>
+        <v>254</v>
+      </c>
+      <c r="K8" s="1">
+        <v>40</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="M8" s="1">
-        <v>40</v>
-      </c>
-      <c r="N8" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2305,26 +2305,26 @@
       <c r="F9" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H9" s="1">
+        <v>60</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q9" t="s">
         <v>257</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="I9" s="1">
-        <v>60</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -2343,38 +2343,38 @@
       <c r="E10" s="1">
         <v>60</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="I10" s="1">
+      <c r="H10" s="1">
         <v>30</v>
       </c>
+      <c r="I10" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="J10" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="K10" t="s">
+        <v>259</v>
+      </c>
+      <c r="K10" s="1">
+        <v>80</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="R10" t="s">
         <v>248</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="M10" s="1">
-        <v>80</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="S10" t="s">
         <v>260</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -2393,35 +2393,35 @@
       <c r="E11" s="1">
         <v>60</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>171</v>
+      </c>
       <c r="H11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="O11" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="R11" t="s">
         <v>261</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="O11" s="1" t="s">
+      <c r="S11" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -2440,38 +2440,38 @@
       <c r="E12" s="1">
         <v>90</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="H12" s="1" t="s">
-        <v>267</v>
+        <v>16</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>16</v>
+        <v>211</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="K12" t="s">
+        <v>266</v>
+      </c>
+      <c r="K12" s="1">
+        <v>20</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="R12" t="s">
         <v>264</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="M12" s="1">
-        <v>20</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="O12" s="1" t="s">
+      <c r="S12" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -2490,35 +2490,35 @@
       <c r="E13" s="1">
         <v>80</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>268</v>
       </c>
+      <c r="I13" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="J13" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="K13" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="K13" s="1">
+        <v>80</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="M13" s="1">
-        <v>80</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="O13" s="1" t="s">
+      <c r="S13" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -2537,38 +2537,38 @@
       <c r="E14" s="1">
         <v>90</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>272</v>
+      </c>
       <c r="H14" s="1" t="s">
-        <v>272</v>
+        <v>16</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>16</v>
+        <v>212</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="K14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="1">
+        <v>40</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="R14" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" s="1">
-        <v>40</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="O14" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -2587,38 +2587,38 @@
       <c r="E15" s="1">
         <v>80</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="I15" s="1">
+      <c r="H15" s="1">
         <v>20</v>
       </c>
+      <c r="I15" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="J15" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="K15" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="K15" s="1">
+        <v>60</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="R15" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="M15" s="1">
-        <v>60</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="O15" s="1" t="s">
+      <c r="S15" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -2640,26 +2640,26 @@
       <c r="F16" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="H16" s="1">
+        <v>60</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q16" t="s">
         <v>281</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="I16" s="1">
-        <v>60</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -2678,38 +2678,38 @@
       <c r="E17" s="1">
         <v>90</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="I17" s="1">
+      <c r="H17" s="1">
         <v>60</v>
       </c>
+      <c r="I17" s="1" t="s">
+        <v>215</v>
+      </c>
       <c r="J17" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="K17" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="K17" s="1">
+        <v>100</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="R17" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="M17" s="1">
-        <v>100</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O17" s="1" t="s">
+      <c r="S17" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="S17" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -2728,38 +2728,38 @@
       <c r="E18" s="1">
         <v>80</v>
       </c>
+      <c r="G18" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="H18" s="1" t="s">
-        <v>285</v>
+        <v>24</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>24</v>
+        <v>202</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="K18" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K18" s="1">
+        <v>40</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="R18" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="M18" s="1">
-        <v>40</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="O18" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -2778,38 +2778,38 @@
       <c r="E19" s="1">
         <v>80</v>
       </c>
+      <c r="G19" s="1" t="s">
+        <v>289</v>
+      </c>
       <c r="H19" s="1" t="s">
-        <v>289</v>
+        <v>24</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>24</v>
+        <v>202</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="K19" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="K19" s="1">
+        <v>20</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="R19" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="M19" s="1">
-        <v>20</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="O19" s="1" t="s">
+      <c r="S19" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="S19" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:19">
@@ -2828,38 +2828,38 @@
       <c r="E20" s="1">
         <v>70</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="I20" s="1">
+      <c r="H20" s="1">
         <v>40</v>
       </c>
+      <c r="I20" s="1" t="s">
+        <v>206</v>
+      </c>
       <c r="J20" s="1" t="s">
-        <v>206</v>
+        <v>292</v>
+      </c>
+      <c r="K20" s="1">
+        <v>70</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="M20" s="1">
-        <v>70</v>
+        <v>190</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="O20" t="s">
+        <v>199</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="S20" t="s">
         <v>293</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="S20" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:19">
@@ -2878,38 +2878,38 @@
       <c r="E21" s="1">
         <v>70</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="I21" s="1">
+      <c r="H21" s="1">
         <v>10</v>
       </c>
+      <c r="I21" s="1" t="s">
+        <v>200</v>
+      </c>
       <c r="J21" s="1" t="s">
-        <v>200</v>
+        <v>295</v>
       </c>
       <c r="K21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="R21" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="O21" t="s">
+      <c r="S21" t="s">
         <v>297</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="S21" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:19">
@@ -2931,29 +2931,29 @@
       <c r="F22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="H22" s="1">
+        <v>50</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q22" t="s">
         <v>298</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="I22" s="1">
-        <v>50</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="K22" s="1" t="s">
+      <c r="R22" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:19">
@@ -2972,38 +2972,38 @@
       <c r="E23" s="1">
         <v>60</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="I23" s="1">
+      <c r="H23" s="1">
         <v>20</v>
       </c>
+      <c r="I23" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="J23" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="K23" t="s">
+        <v>303</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="R23" t="s">
         <v>302</v>
       </c>
-      <c r="L23" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="O23" t="s">
+      <c r="S23" t="s">
         <v>304</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S23" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:19">
@@ -3022,38 +3022,38 @@
       <c r="E24" s="1">
         <v>100</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="I24" s="1">
+      <c r="H24" s="1">
         <v>50</v>
       </c>
+      <c r="I24" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="J24" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="K24" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="K24" s="1">
+        <v>80</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="R24" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="L24" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="M24" s="1">
-        <v>80</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="O24" t="s">
+      <c r="S24" t="s">
         <v>308</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="S24" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -3072,35 +3072,35 @@
       <c r="E25" s="1">
         <v>80</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="I25" s="1">
+      <c r="H25" s="1">
         <v>30</v>
       </c>
+      <c r="I25" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="J25" s="1" t="s">
-        <v>202</v>
+        <v>305</v>
+      </c>
+      <c r="K25" s="1">
+        <v>50</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="M25" s="1">
-        <v>50</v>
-      </c>
-      <c r="N25" s="1" t="s">
         <v>217</v>
       </c>
+      <c r="M25" s="1" t="s">
+        <v>176</v>
+      </c>
       <c r="O25" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S25" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S25" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:19">
@@ -3119,35 +3119,35 @@
       <c r="E26" s="1">
         <v>80</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="I26" s="1">
+      <c r="H26" s="1">
         <v>50</v>
       </c>
+      <c r="I26" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="J26" s="1" t="s">
-        <v>212</v>
+        <v>311</v>
+      </c>
+      <c r="K26" s="1">
+        <v>30</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="M26" s="1">
-        <v>30</v>
-      </c>
-      <c r="N26" s="1" t="s">
         <v>213</v>
       </c>
+      <c r="M26" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="O26" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S26" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="S26" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:19">
@@ -3166,22 +3166,22 @@
       <c r="E27" s="1">
         <v>40</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="I27" s="1">
+      <c r="H27" s="1">
         <v>10</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="N27" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="R27" s="1" t="s">
+      <c r="O27" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="S27" s="2" t="s">
+      <c r="P27" s="2" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3201,38 +3201,38 @@
       <c r="E28" s="1">
         <v>50</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="I28" s="1">
+      <c r="H28" s="1">
         <v>30</v>
       </c>
+      <c r="I28" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="J28" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="K28" s="1">
+        <v>30</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="O28" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="K28" t="s">
+      <c r="P28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="R28" t="s">
         <v>315</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="M28" s="1">
-        <v>30</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S28" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:19">
@@ -3251,22 +3251,22 @@
       <c r="E29" s="1">
         <v>60</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="I29" s="1">
+      <c r="H29" s="1">
         <v>20</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="M29" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="R29" s="1" t="s">
+      <c r="O29" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="S29" s="2" t="s">
+      <c r="P29" s="2" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3286,35 +3286,35 @@
       <c r="E30" s="1">
         <v>60</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>318</v>
       </c>
+      <c r="I30" s="1" t="s">
+        <v>175</v>
+      </c>
       <c r="J30" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="K30" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="K30" s="1">
+        <v>50</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="R30" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="L30" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="M30" s="1">
-        <v>50</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="O30" s="1" t="s">
+      <c r="S30" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S30" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:19">
@@ -3333,35 +3333,35 @@
       <c r="E31" s="1">
         <v>60</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="I31" s="1">
+      <c r="H31" s="1">
         <v>30</v>
       </c>
+      <c r="I31" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="J31" s="1" t="s">
-        <v>211</v>
+        <v>322</v>
+      </c>
+      <c r="K31" s="1">
+        <v>20</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="M31" s="1">
-        <v>20</v>
-      </c>
-      <c r="N31" s="1" t="s">
         <v>193</v>
       </c>
+      <c r="M31" s="1" t="s">
+        <v>183</v>
+      </c>
       <c r="O31" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="S31" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S31" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:19">
@@ -3380,38 +3380,38 @@
       <c r="E32" s="1">
         <v>70</v>
       </c>
+      <c r="G32" s="1" t="s">
+        <v>324</v>
+      </c>
       <c r="H32" s="1" t="s">
-        <v>324</v>
+        <v>40</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>40</v>
+        <v>175</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="K32" t="s">
+        <v>325</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="R32" t="s">
         <v>326</v>
       </c>
-      <c r="L32" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="O32" t="s">
+      <c r="S32" t="s">
         <v>327</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="S32" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:19">
@@ -3430,32 +3430,32 @@
       <c r="E33" s="1">
         <v>60</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="I33" s="1" t="s">
+        <v>174</v>
+      </c>
       <c r="J33" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="K33" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="K33" s="1">
+        <v>50</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="R33" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="M33" s="1">
-        <v>50</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="S33" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:19">
@@ -3474,35 +3474,35 @@
       <c r="E34" s="1">
         <v>80</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>331</v>
       </c>
+      <c r="I34" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="J34" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="K34" t="s">
+        <v>322</v>
+      </c>
+      <c r="K34" s="1">
+        <v>20</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="R34" t="s">
         <v>332</v>
       </c>
-      <c r="L34" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="M34" s="1">
-        <v>20</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="O34" s="1" t="s">
+      <c r="S34" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="R34" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="S34" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:19">
@@ -3521,38 +3521,38 @@
       <c r="E35" s="1">
         <v>80</v>
       </c>
+      <c r="G35" s="1" t="s">
+        <v>333</v>
+      </c>
       <c r="H35" s="1" t="s">
-        <v>333</v>
+        <v>45</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>45</v>
+        <v>206</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="K35" t="s">
+        <v>335</v>
+      </c>
+      <c r="K35" s="1">
+        <v>60</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="R35" t="s">
         <v>334</v>
       </c>
-      <c r="L35" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="M35" s="1">
-        <v>60</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="O35" t="s">
+      <c r="S35" t="s">
         <v>336</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R35" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="S35" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:19">
@@ -3571,35 +3571,35 @@
       <c r="E36" s="1">
         <v>30</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="I36" s="1">
+      <c r="H36" s="1">
         <v>10</v>
       </c>
+      <c r="I36" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="J36" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="O36" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="L36" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="O36" t="s">
+      <c r="P36" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="S36" t="s">
         <v>339</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="R36" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S36" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:19">
@@ -3618,35 +3618,35 @@
       <c r="E37" s="1">
         <v>50</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="I37" s="1">
+      <c r="H37" s="1">
         <v>30</v>
       </c>
+      <c r="I37" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="J37" s="1" t="s">
-        <v>185</v>
+        <v>305</v>
+      </c>
+      <c r="K37" s="1">
+        <v>50</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="M37" s="1">
-        <v>50</v>
-      </c>
-      <c r="N37" s="1" t="s">
         <v>217</v>
       </c>
+      <c r="M37" s="1" t="s">
+        <v>176</v>
+      </c>
       <c r="O37" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="S37" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="P37" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="R37" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="S37" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:19">
@@ -3665,35 +3665,35 @@
       <c r="E38" s="1">
         <v>60</v>
       </c>
+      <c r="G38" s="1" t="s">
+        <v>342</v>
+      </c>
       <c r="H38" s="1" t="s">
-        <v>342</v>
+        <v>24</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>24</v>
+        <v>211</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="K38" t="s">
+        <v>343</v>
+      </c>
+      <c r="K38" s="1">
+        <v>50</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="R38" t="s">
         <v>286</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="M38" s="1">
-        <v>50</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R38" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S38" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:19">
@@ -3712,35 +3712,35 @@
       <c r="E39" s="1">
         <v>60</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="I39" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="J39" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="K39" t="s">
+        <v>324</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="R39" t="s">
         <v>344</v>
       </c>
-      <c r="L39" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N39" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="O39" t="s">
+      <c r="S39" t="s">
         <v>286</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="R39" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S39" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:19">
@@ -3759,35 +3759,35 @@
       <c r="E40" s="1">
         <v>30</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>345</v>
       </c>
+      <c r="I40" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="J40" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="O40" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="K40" t="s">
+      <c r="P40" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="R40" t="s">
         <v>347</v>
       </c>
-      <c r="L40" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="O40" t="s">
+      <c r="S40" t="s">
         <v>348</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="R40" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S40" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:19">
@@ -3806,38 +3806,38 @@
       <c r="E41" s="1">
         <v>60</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="I41" s="1">
+      <c r="H41" s="1">
         <v>20</v>
       </c>
+      <c r="I41" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="J41" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="O41" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="L41" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="O41" t="s">
+      <c r="P41" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="S41" t="s">
         <v>351</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q41" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="R41" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S41" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:19">
@@ -3856,22 +3856,22 @@
       <c r="E42" s="1">
         <v>60</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="I42" s="1">
+      <c r="H42" s="1">
         <v>10</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="P42" s="1" t="s">
+      <c r="M42" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="R42" s="1" t="s">
+      <c r="O42" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="S42" s="2" t="s">
+      <c r="P42" s="2" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3891,32 +3891,32 @@
       <c r="E43" s="1">
         <v>70</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>353</v>
       </c>
+      <c r="I43" s="1" t="s">
+        <v>223</v>
+      </c>
       <c r="J43" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="K43" t="s">
+        <v>349</v>
+      </c>
+      <c r="K43" s="1">
+        <v>40</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P43" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="R43" t="s">
         <v>354</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="M43" s="1">
-        <v>40</v>
-      </c>
-      <c r="N43" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="P43" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="R43" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S43" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:19">
@@ -3935,23 +3935,23 @@
       <c r="E44" s="1">
         <v>30</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="I44" s="1">
+      <c r="H44" s="1">
         <v>10</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="M44" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="R44" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="P44" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="S44" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:19">
@@ -3970,26 +3970,26 @@
       <c r="E45" s="1">
         <v>40</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="I45" s="1">
+      <c r="H45" s="1">
         <v>20</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="K45" t="s">
+      <c r="M45" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="R45" t="s">
         <v>357</v>
-      </c>
-      <c r="P45" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="R45" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S45" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:19">
@@ -4008,26 +4008,26 @@
       <c r="E46" s="1">
         <v>40</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="I46" s="1">
+      <c r="H46" s="1">
         <v>10</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="M46" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="R46" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="P46" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="R46" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S46" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:19">
@@ -4046,35 +4046,35 @@
       <c r="E47" s="1">
         <v>50</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="I47" s="1">
+      <c r="H47" s="1">
         <v>10</v>
       </c>
+      <c r="I47" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="J47" s="1" t="s">
-        <v>225</v>
+        <v>360</v>
+      </c>
+      <c r="K47" s="1">
+        <v>30</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="M47" s="1">
-        <v>30</v>
-      </c>
-      <c r="N47" s="1" t="s">
         <v>219</v>
       </c>
+      <c r="M47" s="1" t="s">
+        <v>176</v>
+      </c>
       <c r="O47" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="S47" s="1" t="s">
         <v>361</v>
-      </c>
-      <c r="P47" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="R47" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S47" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:19">
@@ -4093,31 +4093,31 @@
       <c r="E48" s="1">
         <v>30</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="I48" s="1">
+      <c r="H48" s="1">
         <v>10</v>
       </c>
+      <c r="I48" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="J48" s="1" t="s">
-        <v>189</v>
+        <v>363</v>
+      </c>
+      <c r="K48" s="1">
+        <v>30</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="M48" s="1">
-        <v>30</v>
+        <v>191</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="P48" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q48" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="S48" s="2" t="s">
+      <c r="P48" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -4137,26 +4137,26 @@
       <c r="E49" s="1">
         <v>50</v>
       </c>
+      <c r="G49" s="1" t="s">
+        <v>364</v>
+      </c>
       <c r="H49" s="1" t="s">
-        <v>364</v>
+        <v>40</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J49" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="K49" t="s">
+      <c r="M49" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="R49" t="s">
         <v>326</v>
-      </c>
-      <c r="P49" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q49" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="S49" s="2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:19">
@@ -4175,35 +4175,35 @@
       <c r="E50" s="1">
         <v>50</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="I50" s="1">
+      <c r="H50" s="1">
         <v>10</v>
       </c>
+      <c r="I50" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="J50" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="K50" s="1">
+        <v>10</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O50" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="L50" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="M50" s="1">
-        <v>10</v>
-      </c>
-      <c r="N50" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="O50" s="1" t="s">
+      <c r="P50" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="S50" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="P50" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R50" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S50" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:19">
@@ -4222,29 +4222,29 @@
       <c r="E51" s="1">
         <v>30</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>366</v>
       </c>
+      <c r="I51" s="1" t="s">
+        <v>175</v>
+      </c>
       <c r="J51" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="K51" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="P51" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="R51" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="L51" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="N51" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="O51" s="1" t="s">
+      <c r="S51" s="1" t="s">
         <v>368</v>
-      </c>
-      <c r="Q51" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="S51" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:19">
@@ -4263,26 +4263,26 @@
       <c r="E52" s="1">
         <v>50</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="I52" s="1">
+      <c r="H52" s="1">
         <v>10</v>
       </c>
-      <c r="J52" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="K52" t="s">
+      <c r="M52" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P52" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="R52" t="s">
         <v>370</v>
-      </c>
-      <c r="P52" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R52" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S52" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:19">
@@ -4301,22 +4301,22 @@
       <c r="E53" s="1">
         <v>50</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="I53" s="1">
+      <c r="H53" s="1">
         <v>20</v>
       </c>
-      <c r="J53" s="1" t="s">
+      <c r="I53" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="P53" s="1" t="s">
+      <c r="M53" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="R53" s="1" t="s">
+      <c r="O53" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="S53" s="2" t="s">
+      <c r="P53" s="2" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4336,38 +4336,38 @@
       <c r="E54" s="1">
         <v>40</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="I54" s="1">
+      <c r="H54" s="1">
         <v>10</v>
       </c>
+      <c r="I54" s="1" t="s">
+        <v>200</v>
+      </c>
       <c r="J54" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="K54" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="K54" s="1">
+        <v>40</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="O54" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P54" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="R54" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="L54" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="M54" s="1">
-        <v>40</v>
-      </c>
-      <c r="N54" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="O54" t="s">
+      <c r="S54" t="s">
         <v>372</v>
-      </c>
-      <c r="P54" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="R54" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S54" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:19">
@@ -4386,35 +4386,35 @@
       <c r="E55" s="1">
         <v>70</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="G55" s="1" t="s">
         <v>331</v>
       </c>
+      <c r="I55" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="J55" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="K55" s="1">
+        <v>20</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O55" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="K55" t="s">
+      <c r="P55" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="R55" t="s">
         <v>373</v>
       </c>
-      <c r="L55" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="M55" s="1">
-        <v>20</v>
-      </c>
-      <c r="N55" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="O55" s="1" t="s">
+      <c r="S55" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="P55" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="R55" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="S55" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:19">
@@ -4433,26 +4433,26 @@
       <c r="E56" s="1">
         <v>40</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="G56" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="I56" s="1">
+      <c r="H56" s="1">
         <v>30</v>
       </c>
-      <c r="J56" s="1" t="s">
+      <c r="I56" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="K56" t="s">
+      <c r="M56" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P56" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="R56" t="s">
         <v>376</v>
-      </c>
-      <c r="P56" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R56" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S56" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:19">
@@ -4471,32 +4471,32 @@
       <c r="E57" s="1">
         <v>90</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="G57" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="I57" s="1">
+      <c r="H57" s="1">
         <v>10</v>
       </c>
+      <c r="I57" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="J57" s="1" t="s">
-        <v>189</v>
+        <v>378</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="N57" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="O57" t="s">
+      <c r="M57" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P57" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="S57" t="s">
         <v>379</v>
-      </c>
-      <c r="P57" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="R57" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="S57" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:19">
@@ -4515,29 +4515,29 @@
       <c r="E58" s="1">
         <v>40</v>
       </c>
-      <c r="H58" s="1" t="s">
+      <c r="G58" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="I58" s="1">
+      <c r="H58" s="1">
         <v>10</v>
       </c>
-      <c r="J58" s="1" t="s">
+      <c r="I58" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="K58" s="1" t="s">
+      <c r="M58" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P58" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="R58" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="P58" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q58" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="R58" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S58" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:19">
@@ -4556,35 +4556,35 @@
       <c r="E59" s="1">
         <v>40</v>
       </c>
-      <c r="H59" s="1" t="s">
+      <c r="G59" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="I59" s="1">
+      <c r="H59" s="1">
         <v>10</v>
       </c>
+      <c r="I59" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="J59" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="K59" s="1">
+        <v>30</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="O59" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="L59" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="M59" s="1">
-        <v>30</v>
-      </c>
-      <c r="N59" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="O59" t="s">
+      <c r="P59" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="S59" t="s">
         <v>383</v>
-      </c>
-      <c r="P59" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="R59" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S59" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:19">
@@ -4603,26 +4603,26 @@
       <c r="E60" s="1">
         <v>40</v>
       </c>
+      <c r="G60" s="1" t="s">
+        <v>272</v>
+      </c>
       <c r="H60" s="1" t="s">
-        <v>272</v>
+        <v>14</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J60" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="K60" s="1" t="s">
+      <c r="M60" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P60" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="R60" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="P60" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="R60" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S60" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:19">
@@ -4641,31 +4641,31 @@
       <c r="E61" s="1">
         <v>40</v>
       </c>
-      <c r="H61" s="1" t="s">
+      <c r="G61" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="I61" s="1">
+      <c r="H61" s="1">
         <v>20</v>
       </c>
+      <c r="I61" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="J61" s="1" t="s">
-        <v>203</v>
+        <v>386</v>
+      </c>
+      <c r="K61" s="1">
+        <v>30</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="M61" s="1">
-        <v>30</v>
-      </c>
-      <c r="N61" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="P61" s="1" t="s">
+      <c r="M61" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="R61" s="1" t="s">
+      <c r="O61" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="S61" s="2" t="s">
+      <c r="P61" s="2" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4685,22 +4685,22 @@
       <c r="E62" s="1">
         <v>30</v>
       </c>
-      <c r="H62" s="1" t="s">
+      <c r="G62" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="I62" s="1">
+      <c r="H62" s="1">
         <v>20</v>
       </c>
-      <c r="J62" s="1" t="s">
+      <c r="I62" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="P62" s="1" t="s">
+      <c r="M62" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="Q62" s="1" t="s">
+      <c r="N62" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="S62" s="2" t="s">
+      <c r="P62" s="2" t="s">
         <v>142</v>
       </c>
     </row>
@@ -4720,29 +4720,29 @@
       <c r="E63" s="1">
         <v>40</v>
       </c>
-      <c r="H63" s="1" t="s">
+      <c r="G63" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="I63" s="1">
+      <c r="H63" s="1">
         <v>10</v>
       </c>
-      <c r="J63" s="1" t="s">
+      <c r="I63" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="K63" t="s">
+      <c r="M63" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="O63" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P63" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="R63" t="s">
         <v>388</v>
-      </c>
-      <c r="P63" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q63" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="R63" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S63" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="64" spans="1:19">
@@ -4761,35 +4761,35 @@
       <c r="E64" s="1">
         <v>40</v>
       </c>
-      <c r="H64" s="1" t="s">
+      <c r="G64" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="I64" s="1">
+      <c r="H64" s="1">
         <v>10</v>
       </c>
+      <c r="I64" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="J64" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="K64" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="O64" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P64" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="R64" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="L64" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="N64" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="O64" t="s">
+      <c r="S64" t="s">
         <v>390</v>
-      </c>
-      <c r="P64" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="R64" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S64" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="65" spans="1:19">
@@ -4808,35 +4808,35 @@
       <c r="E65" s="1">
         <v>60</v>
       </c>
-      <c r="H65" s="1" t="s">
+      <c r="G65" s="1" t="s">
         <v>328</v>
       </c>
+      <c r="I65" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="J65" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="K65" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="K65" s="1">
+        <v>20</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="O65" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P65" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="R65" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="L65" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="M65" s="1">
-        <v>20</v>
-      </c>
-      <c r="N65" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="O65" s="1" t="s">
+      <c r="S65" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="P65" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="R65" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S65" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="66" spans="1:19">
@@ -4855,22 +4855,22 @@
       <c r="E66" s="1">
         <v>40</v>
       </c>
-      <c r="H66" s="1" t="s">
+      <c r="G66" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="I66" s="1">
+      <c r="H66" s="1">
         <v>20</v>
       </c>
-      <c r="J66" s="1" t="s">
+      <c r="I66" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="P66" s="1" t="s">
+      <c r="M66" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="R66" s="1" t="s">
+      <c r="O66" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="S66" s="2" t="s">
+      <c r="P66" s="2" t="s">
         <v>146</v>
       </c>
     </row>
@@ -4890,38 +4890,38 @@
       <c r="E67" s="1">
         <v>50</v>
       </c>
-      <c r="H67" s="1" t="s">
+      <c r="G67" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="I67" s="1">
+      <c r="H67" s="1">
         <v>20</v>
       </c>
+      <c r="I67" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="J67" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="K67" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="K67" s="1">
+        <v>20</v>
+      </c>
+      <c r="L67" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O67" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="P67" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="R67" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="L67" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="M67" s="1">
-        <v>20</v>
-      </c>
-      <c r="N67" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="O67" s="1" t="s">
+      <c r="S67" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="P67" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="R67" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="S67" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="68" spans="1:19">
@@ -4940,22 +4940,22 @@
       <c r="E68" s="1">
         <v>40</v>
       </c>
-      <c r="H68" s="1" t="s">
+      <c r="G68" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="I68" s="1">
+      <c r="H68" s="1">
         <v>10</v>
       </c>
-      <c r="J68" s="1" t="s">
+      <c r="I68" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="P68" s="1" t="s">
+      <c r="M68" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="R68" s="1" t="s">
+      <c r="O68" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="S68" s="2" t="s">
+      <c r="P68" s="2" t="s">
         <v>148</v>
       </c>
     </row>
@@ -4975,26 +4975,26 @@
       <c r="E69" s="1">
         <v>50</v>
       </c>
-      <c r="H69" s="1" t="s">
+      <c r="G69" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="I69" s="1">
+      <c r="H69" s="1">
         <v>10</v>
       </c>
-      <c r="J69" s="1" t="s">
+      <c r="I69" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="K69" s="1" t="s">
+      <c r="M69" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="O69" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P69" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="R69" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="P69" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="R69" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S69" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:19">
@@ -5013,99 +5013,99 @@
       <c r="E70" s="1">
         <v>40</v>
       </c>
-      <c r="H70" s="1" t="s">
+      <c r="G70" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="I70" s="1">
+      <c r="H70" s="1">
         <v>10</v>
       </c>
-      <c r="J70" s="1" t="s">
+      <c r="I70" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="K70" s="1" t="s">
+      <c r="M70" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O70" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="P70" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="R70" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="P70" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="R70" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="S70" s="2" t="s">
-        <v>150</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1" xr:uid="{BAA56797-48E0-4455-84D7-888584FAD678}"/>
-    <hyperlink ref="S5" r:id="rId2" xr:uid="{14C2C412-1F3B-4DC6-A89C-71FA2AD5C5BE}"/>
-    <hyperlink ref="S9" r:id="rId3" xr:uid="{05CFD655-7069-44F9-A1B6-157C121B8863}"/>
-    <hyperlink ref="S10" r:id="rId4" xr:uid="{AD3DAF43-9348-4C6D-8F18-55126B45AC50}"/>
-    <hyperlink ref="S11" r:id="rId5" xr:uid="{748F4BE9-0063-4D2F-973E-39578DD327D7}"/>
-    <hyperlink ref="S15" r:id="rId6" xr:uid="{89EE3067-B701-495A-8258-DCF6BF941F83}"/>
-    <hyperlink ref="S16" r:id="rId7" xr:uid="{833D3E65-B723-4FA2-BD90-C73E3EBC37D3}"/>
-    <hyperlink ref="S17" r:id="rId8" xr:uid="{9E26B95E-46E6-4276-9DC6-5694A11CF9D5}"/>
-    <hyperlink ref="S18" r:id="rId9" xr:uid="{4F75B442-7086-47B6-B0C4-2581D22D0EEF}"/>
-    <hyperlink ref="S19" r:id="rId10" xr:uid="{5FCDC780-7C18-4C70-B8A9-A228C26EC755}"/>
-    <hyperlink ref="S20" r:id="rId11" xr:uid="{4C5BC5BD-022C-455C-86EC-F7BE2C63CDA1}"/>
-    <hyperlink ref="S21" r:id="rId12" xr:uid="{CFD80C7B-31C7-43B1-9D3B-D33B597C56DD}"/>
-    <hyperlink ref="S22" r:id="rId13" xr:uid="{92BA6329-13BE-43CE-9F24-C1D90E1B1951}"/>
-    <hyperlink ref="S23" r:id="rId14" xr:uid="{352DD5F1-B1DF-4219-ACFE-8EB822B043EA}"/>
-    <hyperlink ref="S24" r:id="rId15" xr:uid="{CC97B808-0792-499B-BE0A-187783585569}"/>
-    <hyperlink ref="S25" r:id="rId16" xr:uid="{EF7EBC88-43F5-46EB-BCB9-0E46368278A3}"/>
-    <hyperlink ref="S27" r:id="rId17" xr:uid="{B8AECA6C-B5A5-4DAA-8C38-D013CCBD57F8}"/>
-    <hyperlink ref="S26" r:id="rId18" xr:uid="{49CB4665-4F62-4C9F-97AF-77B9E6AC13C3}"/>
-    <hyperlink ref="S14" r:id="rId19" xr:uid="{D451CC42-1475-427C-9A53-6833B93E1F3A}"/>
-    <hyperlink ref="S13" r:id="rId20" xr:uid="{9B55965A-F225-4527-8B02-EBC5E8715085}"/>
-    <hyperlink ref="S12" r:id="rId21" xr:uid="{2A75C111-63C5-4C38-BC81-FF95035E4EB1}"/>
-    <hyperlink ref="S8" r:id="rId22" xr:uid="{E9C232B1-5153-4522-876E-C3C9F1F77095}"/>
-    <hyperlink ref="S7" r:id="rId23" xr:uid="{6D15494E-2F51-4720-AFBC-507C1CAD6257}"/>
-    <hyperlink ref="S6" r:id="rId24" xr:uid="{5BBCDBA6-D705-4EFF-BE0F-B10A145BE864}"/>
-    <hyperlink ref="S4" r:id="rId25" xr:uid="{18726A41-E92A-45AD-B7BB-7036BA6F5062}"/>
-    <hyperlink ref="S3" r:id="rId26" xr:uid="{BD5B4C9F-A269-40FD-801F-499CB3C1ADCC}"/>
-    <hyperlink ref="S28" r:id="rId27" xr:uid="{1E0C87A4-7920-4F06-9AAD-FDD1FB4214D1}"/>
-    <hyperlink ref="S29" r:id="rId28" xr:uid="{96DE1B79-13C7-4CCF-862A-417B0CE63275}"/>
-    <hyperlink ref="S30" r:id="rId29" xr:uid="{3B11749C-4683-470D-AFBA-685128FA512D}"/>
-    <hyperlink ref="S31" r:id="rId30" xr:uid="{4F19AB1A-8F4E-43CC-BB1E-EBEB46B8CE98}"/>
-    <hyperlink ref="S32" r:id="rId31" xr:uid="{712AB733-2432-4AB4-82AD-919327188942}"/>
-    <hyperlink ref="S34" r:id="rId32" xr:uid="{3E1CDC9E-18AA-48D4-B607-2B94A0B6B20A}"/>
-    <hyperlink ref="S33" r:id="rId33" xr:uid="{1B212F92-C147-4EA0-856B-402969CEFE0C}"/>
-    <hyperlink ref="S35" r:id="rId34" xr:uid="{F8E12793-7E9F-4D52-89DF-D6EA8777BDBB}"/>
-    <hyperlink ref="S36" r:id="rId35" xr:uid="{F74C04AB-B785-4A56-978D-A0FA5EA7E943}"/>
-    <hyperlink ref="S37" r:id="rId36" xr:uid="{176C87F9-C32E-4BD8-9A3E-68BA707D64C3}"/>
-    <hyperlink ref="S38" r:id="rId37" xr:uid="{35F70388-137F-4BE1-A3E7-B37D6AB4A90C}"/>
-    <hyperlink ref="S39" r:id="rId38" xr:uid="{7FF3C9A7-23DD-46CF-8F10-F1359E422BB1}"/>
-    <hyperlink ref="S40" r:id="rId39" xr:uid="{A41C2C7B-E193-4B41-A9A2-ABFF261129BD}"/>
-    <hyperlink ref="S41" r:id="rId40" xr:uid="{7B015720-4785-4125-83FD-A90685F4B924}"/>
-    <hyperlink ref="S42" r:id="rId41" xr:uid="{80F30380-2EAB-4A95-BF02-173787F44A16}"/>
-    <hyperlink ref="S43" r:id="rId42" xr:uid="{7BE75EB4-773F-4313-B65F-68102CA9A730}"/>
-    <hyperlink ref="S44" r:id="rId43" xr:uid="{16BF42C8-9E71-4469-9B25-929FBBBF8A64}"/>
-    <hyperlink ref="S45" r:id="rId44" xr:uid="{DD1DDDE3-2F39-442D-87F1-CB1C4FCF10E0}"/>
-    <hyperlink ref="S46" r:id="rId45" xr:uid="{0062BE15-118A-4D98-AF18-C0CA4E1B8B14}"/>
-    <hyperlink ref="S49" r:id="rId46" xr:uid="{5DFAA0D3-D5CB-4961-AF86-E9F42D3D31C0}"/>
-    <hyperlink ref="S50" r:id="rId47" xr:uid="{2EE21BF1-064F-4176-B1B5-35A00C462CD8}"/>
-    <hyperlink ref="S51" r:id="rId48" xr:uid="{F79F7423-7F42-4272-B725-63CF80511099}"/>
-    <hyperlink ref="S52" r:id="rId49" xr:uid="{20947250-C792-4310-9A7E-18CA52D326D8}"/>
-    <hyperlink ref="S53" r:id="rId50" xr:uid="{C97D8CCB-019A-4CC6-8D06-CA01F780E025}"/>
-    <hyperlink ref="S54" r:id="rId51" xr:uid="{110228AF-19FD-4DA6-8C85-DB31B7EBE845}"/>
-    <hyperlink ref="S55" r:id="rId52" xr:uid="{F33B812A-0DC1-4604-9E79-09FA8C5A6D3E}"/>
-    <hyperlink ref="S56" r:id="rId53" xr:uid="{E157632E-EC42-43C6-995B-2AA9D7BB8936}"/>
-    <hyperlink ref="S57" r:id="rId54" xr:uid="{8116F1BC-B851-4541-BD7E-FDE4B6C25446}"/>
-    <hyperlink ref="S58" r:id="rId55" xr:uid="{F5FFBFD3-B26B-463F-8FDA-7430B5AD1FBD}"/>
-    <hyperlink ref="S59" r:id="rId56" xr:uid="{B38A678F-E289-407D-9602-2DB1BB12DF45}"/>
-    <hyperlink ref="S60" r:id="rId57" xr:uid="{F2F57B8E-14AD-472E-A331-699956FF2821}"/>
-    <hyperlink ref="S61" r:id="rId58" xr:uid="{A6AE4C62-F3FE-4EEC-98E3-A1E63421600E}"/>
-    <hyperlink ref="S62" r:id="rId59" xr:uid="{674F707F-19F0-4C18-8EDA-9551FBC10C32}"/>
-    <hyperlink ref="S63" r:id="rId60" xr:uid="{1410175B-1152-4E46-8604-A2F77C0D9505}"/>
-    <hyperlink ref="S64" r:id="rId61" xr:uid="{50C6456B-4CD4-47D0-AB1A-AD11349186B9}"/>
-    <hyperlink ref="S65" r:id="rId62" xr:uid="{AAD99EE2-B6D3-43EB-9B7E-4EAD389F3F14}"/>
-    <hyperlink ref="S66" r:id="rId63" xr:uid="{12699A7D-8DB7-480C-9C1A-8CB8438DBBC6}"/>
-    <hyperlink ref="S68" r:id="rId64" xr:uid="{32C03333-51F1-4217-8234-73AC84F29B1E}"/>
-    <hyperlink ref="S70" r:id="rId65" xr:uid="{382A628E-6712-4E8F-A7A5-6DD9BAE70C51}"/>
-    <hyperlink ref="S69" r:id="rId66" xr:uid="{04C1BBF5-73C9-4E1C-B08C-B0B633803133}"/>
-    <hyperlink ref="S67" r:id="rId67" xr:uid="{2E5D21A1-B685-469F-8FDB-8A65D31B5E18}"/>
-    <hyperlink ref="S48" r:id="rId68" xr:uid="{7F50E082-0243-48F8-9DAD-488B0C94219D}"/>
-    <hyperlink ref="S47" r:id="rId69" xr:uid="{489AFE98-0257-4B10-8283-01EAD0817C73}"/>
+    <hyperlink ref="P2" r:id="rId1" xr:uid="{BAA56797-48E0-4455-84D7-888584FAD678}"/>
+    <hyperlink ref="P5" r:id="rId2" xr:uid="{14C2C412-1F3B-4DC6-A89C-71FA2AD5C5BE}"/>
+    <hyperlink ref="P9" r:id="rId3" xr:uid="{05CFD655-7069-44F9-A1B6-157C121B8863}"/>
+    <hyperlink ref="P10" r:id="rId4" xr:uid="{AD3DAF43-9348-4C6D-8F18-55126B45AC50}"/>
+    <hyperlink ref="P11" r:id="rId5" xr:uid="{748F4BE9-0063-4D2F-973E-39578DD327D7}"/>
+    <hyperlink ref="P15" r:id="rId6" xr:uid="{89EE3067-B701-495A-8258-DCF6BF941F83}"/>
+    <hyperlink ref="P16" r:id="rId7" xr:uid="{833D3E65-B723-4FA2-BD90-C73E3EBC37D3}"/>
+    <hyperlink ref="P17" r:id="rId8" xr:uid="{9E26B95E-46E6-4276-9DC6-5694A11CF9D5}"/>
+    <hyperlink ref="P18" r:id="rId9" xr:uid="{4F75B442-7086-47B6-B0C4-2581D22D0EEF}"/>
+    <hyperlink ref="P19" r:id="rId10" xr:uid="{5FCDC780-7C18-4C70-B8A9-A228C26EC755}"/>
+    <hyperlink ref="P20" r:id="rId11" xr:uid="{4C5BC5BD-022C-455C-86EC-F7BE2C63CDA1}"/>
+    <hyperlink ref="P21" r:id="rId12" xr:uid="{CFD80C7B-31C7-43B1-9D3B-D33B597C56DD}"/>
+    <hyperlink ref="P22" r:id="rId13" xr:uid="{92BA6329-13BE-43CE-9F24-C1D90E1B1951}"/>
+    <hyperlink ref="P23" r:id="rId14" xr:uid="{352DD5F1-B1DF-4219-ACFE-8EB822B043EA}"/>
+    <hyperlink ref="P24" r:id="rId15" xr:uid="{CC97B808-0792-499B-BE0A-187783585569}"/>
+    <hyperlink ref="P25" r:id="rId16" xr:uid="{EF7EBC88-43F5-46EB-BCB9-0E46368278A3}"/>
+    <hyperlink ref="P27" r:id="rId17" xr:uid="{B8AECA6C-B5A5-4DAA-8C38-D013CCBD57F8}"/>
+    <hyperlink ref="P26" r:id="rId18" xr:uid="{49CB4665-4F62-4C9F-97AF-77B9E6AC13C3}"/>
+    <hyperlink ref="P14" r:id="rId19" xr:uid="{D451CC42-1475-427C-9A53-6833B93E1F3A}"/>
+    <hyperlink ref="P13" r:id="rId20" xr:uid="{9B55965A-F225-4527-8B02-EBC5E8715085}"/>
+    <hyperlink ref="P12" r:id="rId21" xr:uid="{2A75C111-63C5-4C38-BC81-FF95035E4EB1}"/>
+    <hyperlink ref="P8" r:id="rId22" xr:uid="{E9C232B1-5153-4522-876E-C3C9F1F77095}"/>
+    <hyperlink ref="P7" r:id="rId23" xr:uid="{6D15494E-2F51-4720-AFBC-507C1CAD6257}"/>
+    <hyperlink ref="P6" r:id="rId24" xr:uid="{5BBCDBA6-D705-4EFF-BE0F-B10A145BE864}"/>
+    <hyperlink ref="P4" r:id="rId25" xr:uid="{18726A41-E92A-45AD-B7BB-7036BA6F5062}"/>
+    <hyperlink ref="P3" r:id="rId26" xr:uid="{BD5B4C9F-A269-40FD-801F-499CB3C1ADCC}"/>
+    <hyperlink ref="P28" r:id="rId27" xr:uid="{1E0C87A4-7920-4F06-9AAD-FDD1FB4214D1}"/>
+    <hyperlink ref="P29" r:id="rId28" xr:uid="{96DE1B79-13C7-4CCF-862A-417B0CE63275}"/>
+    <hyperlink ref="P30" r:id="rId29" xr:uid="{3B11749C-4683-470D-AFBA-685128FA512D}"/>
+    <hyperlink ref="P31" r:id="rId30" xr:uid="{4F19AB1A-8F4E-43CC-BB1E-EBEB46B8CE98}"/>
+    <hyperlink ref="P32" r:id="rId31" xr:uid="{712AB733-2432-4AB4-82AD-919327188942}"/>
+    <hyperlink ref="P34" r:id="rId32" xr:uid="{3E1CDC9E-18AA-48D4-B607-2B94A0B6B20A}"/>
+    <hyperlink ref="P33" r:id="rId33" xr:uid="{1B212F92-C147-4EA0-856B-402969CEFE0C}"/>
+    <hyperlink ref="P35" r:id="rId34" xr:uid="{F8E12793-7E9F-4D52-89DF-D6EA8777BDBB}"/>
+    <hyperlink ref="P36" r:id="rId35" xr:uid="{F74C04AB-B785-4A56-978D-A0FA5EA7E943}"/>
+    <hyperlink ref="P37" r:id="rId36" xr:uid="{176C87F9-C32E-4BD8-9A3E-68BA707D64C3}"/>
+    <hyperlink ref="P38" r:id="rId37" xr:uid="{35F70388-137F-4BE1-A3E7-B37D6AB4A90C}"/>
+    <hyperlink ref="P39" r:id="rId38" xr:uid="{7FF3C9A7-23DD-46CF-8F10-F1359E422BB1}"/>
+    <hyperlink ref="P40" r:id="rId39" xr:uid="{A41C2C7B-E193-4B41-A9A2-ABFF261129BD}"/>
+    <hyperlink ref="P41" r:id="rId40" xr:uid="{7B015720-4785-4125-83FD-A90685F4B924}"/>
+    <hyperlink ref="P42" r:id="rId41" xr:uid="{80F30380-2EAB-4A95-BF02-173787F44A16}"/>
+    <hyperlink ref="P43" r:id="rId42" xr:uid="{7BE75EB4-773F-4313-B65F-68102CA9A730}"/>
+    <hyperlink ref="P44" r:id="rId43" xr:uid="{16BF42C8-9E71-4469-9B25-929FBBBF8A64}"/>
+    <hyperlink ref="P45" r:id="rId44" xr:uid="{DD1DDDE3-2F39-442D-87F1-CB1C4FCF10E0}"/>
+    <hyperlink ref="P46" r:id="rId45" xr:uid="{0062BE15-118A-4D98-AF18-C0CA4E1B8B14}"/>
+    <hyperlink ref="P49" r:id="rId46" xr:uid="{5DFAA0D3-D5CB-4961-AF86-E9F42D3D31C0}"/>
+    <hyperlink ref="P50" r:id="rId47" xr:uid="{2EE21BF1-064F-4176-B1B5-35A00C462CD8}"/>
+    <hyperlink ref="P51" r:id="rId48" xr:uid="{F79F7423-7F42-4272-B725-63CF80511099}"/>
+    <hyperlink ref="P52" r:id="rId49" xr:uid="{20947250-C792-4310-9A7E-18CA52D326D8}"/>
+    <hyperlink ref="P53" r:id="rId50" xr:uid="{C97D8CCB-019A-4CC6-8D06-CA01F780E025}"/>
+    <hyperlink ref="P54" r:id="rId51" xr:uid="{110228AF-19FD-4DA6-8C85-DB31B7EBE845}"/>
+    <hyperlink ref="P55" r:id="rId52" xr:uid="{F33B812A-0DC1-4604-9E79-09FA8C5A6D3E}"/>
+    <hyperlink ref="P56" r:id="rId53" xr:uid="{E157632E-EC42-43C6-995B-2AA9D7BB8936}"/>
+    <hyperlink ref="P57" r:id="rId54" xr:uid="{8116F1BC-B851-4541-BD7E-FDE4B6C25446}"/>
+    <hyperlink ref="P58" r:id="rId55" xr:uid="{F5FFBFD3-B26B-463F-8FDA-7430B5AD1FBD}"/>
+    <hyperlink ref="P59" r:id="rId56" xr:uid="{B38A678F-E289-407D-9602-2DB1BB12DF45}"/>
+    <hyperlink ref="P60" r:id="rId57" xr:uid="{F2F57B8E-14AD-472E-A331-699956FF2821}"/>
+    <hyperlink ref="P61" r:id="rId58" xr:uid="{A6AE4C62-F3FE-4EEC-98E3-A1E63421600E}"/>
+    <hyperlink ref="P62" r:id="rId59" xr:uid="{674F707F-19F0-4C18-8EDA-9551FBC10C32}"/>
+    <hyperlink ref="P63" r:id="rId60" xr:uid="{1410175B-1152-4E46-8604-A2F77C0D9505}"/>
+    <hyperlink ref="P64" r:id="rId61" xr:uid="{50C6456B-4CD4-47D0-AB1A-AD11349186B9}"/>
+    <hyperlink ref="P65" r:id="rId62" xr:uid="{AAD99EE2-B6D3-43EB-9B7E-4EAD389F3F14}"/>
+    <hyperlink ref="P66" r:id="rId63" xr:uid="{12699A7D-8DB7-480C-9C1A-8CB8438DBBC6}"/>
+    <hyperlink ref="P68" r:id="rId64" xr:uid="{32C03333-51F1-4217-8234-73AC84F29B1E}"/>
+    <hyperlink ref="P70" r:id="rId65" xr:uid="{382A628E-6712-4E8F-A7A5-6DD9BAE70C51}"/>
+    <hyperlink ref="P69" r:id="rId66" xr:uid="{04C1BBF5-73C9-4E1C-B08C-B0B633803133}"/>
+    <hyperlink ref="P67" r:id="rId67" xr:uid="{2E5D21A1-B685-469F-8FDB-8A65D31B5E18}"/>
+    <hyperlink ref="P48" r:id="rId68" xr:uid="{7F50E082-0243-48F8-9DAD-488B0C94219D}"/>
+    <hyperlink ref="P47" r:id="rId69" xr:uid="{489AFE98-0257-4B10-8283-01EAD0817C73}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId70"/>

</xml_diff>